<commit_message>
Add tcr analysis test data
</commit_message>
<xml_diff>
--- a/template_examples/tcr_analysis_template.xlsx
+++ b/template_examples/tcr_analysis_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E4E1AF-6C17-4E47-960E-08B8B849B019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0A585A-F966-C741-A09D-C6514BDBCC71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="1360" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCRseq Analysis" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -99,21 +99,12 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Path to a file on a user's computer.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In .csv format</t>
+          <t>Path to a file on a user's computer.
+In .csv format</t>
         </r>
       </text>
     </comment>
@@ -166,10 +157,10 @@
     <t>E.g. 'CTTTP01A1.00'</t>
   </si>
   <si>
-    <t>Tra clones</t>
-  </si>
-  <si>
-    <t>Trb clones</t>
+    <t>Tra clone</t>
+  </si>
+  <si>
+    <t>Trb clone</t>
   </si>
   <si>
     <t>#t</t>
@@ -190,6 +181,24 @@
     <t>#d</t>
   </si>
   <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>tra_clones_count_1.csv</t>
+  </si>
+  <si>
+    <t>trb_clones_count_1.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>tra_clones_count_2.csv</t>
+  </si>
+  <si>
+    <t>trb_clones_count_2.csv</t>
+  </si>
+  <si>
     <t>test_prism_trial_id</t>
   </si>
   <si>
@@ -197,31 +206,13 @@
   </si>
   <si>
     <t>summary_info.csv</t>
-  </si>
-  <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>tra_clones_count_1.csv</t>
-  </si>
-  <si>
-    <t>trb_clones_count_1.csv</t>
-  </si>
-  <si>
-    <t>tra_clones_count_2.csv</t>
-  </si>
-  <si>
-    <t>trb_clones_count_2.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,12 +231,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -678,7 +663,7 @@
   <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -687,7 +672,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -696,7 +681,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -704,10 +689,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -715,7 +700,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -726,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -755,13 +740,13 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -769,13 +754,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix TRA TRB names
</commit_message>
<xml_diff>
--- a/template_examples/tcr_analysis_template.xlsx
+++ b/template_examples/tcr_analysis_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0A585A-F966-C741-A09D-C6514BDBCC71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3B82D9-5C81-9A47-91DB-51E6613FB990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,10 +157,10 @@
     <t>E.g. 'CTTTP01A1.00'</t>
   </si>
   <si>
-    <t>Tra clone</t>
-  </si>
-  <si>
-    <t>Trb clone</t>
+    <t>Tra clones umi counts</t>
+  </si>
+  <si>
+    <t>Trb clones umi counts</t>
   </si>
   <si>
     <t>#t</t>
@@ -184,21 +184,9 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>tra_clones_count_1.csv</t>
-  </si>
-  <si>
-    <t>trb_clones_count_1.csv</t>
-  </si>
-  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>tra_clones_count_2.csv</t>
-  </si>
-  <si>
-    <t>trb_clones_count_2.csv</t>
-  </si>
-  <si>
     <t>test_prism_trial_id</t>
   </si>
   <si>
@@ -206,6 +194,18 @@
   </si>
   <si>
     <t>summary_info.csv</t>
+  </si>
+  <si>
+    <t>1A_10_0_TRA_clones_umi_count.csv</t>
+  </si>
+  <si>
+    <t>1A_10_0_TRB_clones_umi_count.csv</t>
+  </si>
+  <si>
+    <t>2A_10_0_TRA_clones_umi_count.csv</t>
+  </si>
+  <si>
+    <t>2A_10_0_TRB_clones_umi_count.csv</t>
   </si>
 </sst>
 </file>
@@ -267,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -301,11 +301,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -317,6 +343,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -663,7 +695,7 @@
   <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -672,16 +704,16 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -689,10 +721,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -700,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -711,15 +743,15 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -743,10 +775,10 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -754,13 +786,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1759,6 +1791,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix TCR analysis example data
</commit_message>
<xml_diff>
--- a/template_examples/tcr_analysis_template.xlsx
+++ b/template_examples/tcr_analysis_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5FD8DC-C598-8C46-A508-697BC8D21619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BA2DA4-7711-A74D-B615-6BC454426EE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCRseq Analysis" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
   <dimension ref="A1:D2008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>